<commit_message>
extract vb macros from absGlyphList.xlsx
This and previous name change so we don't have to have macros enabled on that spreadsheet.
</commit_message>
<xml_diff>
--- a/absGlyphList/absGlyphList.xlsx
+++ b/absGlyphList/absGlyphList.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420" codeName="{7A2D7E96-6E34-419A-AE5F-296B3A7E7977}"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr date1904="1" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -16,7 +16,6 @@
     <sheet name="Contextual alignment" sheetId="2" r:id="rId2"/>
     <sheet name="ShapeOrderOriginal" sheetId="3" r:id="rId3"/>
   </sheets>
-  <functionGroups builtInGroupCount="18"/>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">absGlyphList!$A$1:$X$1483</definedName>
   </definedNames>
@@ -8439,7 +8438,7 @@
     <t>not found</t>
   </si>
   <si>
-    <t>Becca'sOrder</t>
+    <t>DesignerOrder</t>
   </si>
 </sst>
 </file>
@@ -9207,7 +9206,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add Persian digits to Harmattan
</commit_message>
<xml_diff>
--- a/absGlyphList/absGlyphList.xlsx
+++ b/absGlyphList/absGlyphList.xlsx
@@ -15417,16 +15417,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr transitionEvaluation="1" codeName="Sheet1" filterMode="1">
+  <sheetPr transitionEvaluation="1" codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AB1582"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B514" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1217" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B569" sqref="B569"/>
+      <selection pane="bottomRight" activeCell="J1251" sqref="J1251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15666,7 +15666,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="5" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>1020</v>
       </c>
@@ -15818,7 +15818,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>249</v>
       </c>
@@ -16074,7 +16074,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
         <v>486</v>
       </c>
@@ -16141,7 +16141,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>487</v>
       </c>
@@ -16205,7 +16205,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>488</v>
       </c>
@@ -17447,7 +17447,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A60" s="19" t="s">
         <v>258</v>
       </c>
@@ -24185,7 +24185,7 @@
         <v>3318.0510000000004</v>
       </c>
     </row>
-    <row r="251" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A251" s="19" t="s">
         <v>4822</v>
       </c>
@@ -24232,7 +24232,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="252" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A252" s="19" t="s">
         <v>4823</v>
       </c>
@@ -24537,7 +24537,7 @@
         <v>3321.0510000000004</v>
       </c>
     </row>
-    <row r="259" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A259" s="19" t="s">
         <v>461</v>
       </c>
@@ -24581,7 +24581,7 @@
         <v>3324</v>
       </c>
     </row>
-    <row r="260" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A260" s="19" t="s">
         <v>689</v>
       </c>
@@ -24622,7 +24622,7 @@
         <v>3324.0010000000002</v>
       </c>
     </row>
-    <row r="261" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A261" s="19" t="s">
         <v>1235</v>
       </c>
@@ -24663,7 +24663,7 @@
         <v>3324.0310000000004</v>
       </c>
     </row>
-    <row r="262" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A262" s="19" t="s">
         <v>1206</v>
       </c>
@@ -24704,7 +24704,7 @@
         <v>3324.0410000000002</v>
       </c>
     </row>
-    <row r="263" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A263" s="19" t="s">
         <v>231</v>
       </c>
@@ -24748,7 +24748,7 @@
         <v>3325</v>
       </c>
     </row>
-    <row r="264" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A264" s="19" t="s">
         <v>690</v>
       </c>
@@ -24789,7 +24789,7 @@
         <v>3325.0010000000002</v>
       </c>
     </row>
-    <row r="265" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A265" s="19" t="s">
         <v>1236</v>
       </c>
@@ -24830,7 +24830,7 @@
         <v>3325.0310000000004</v>
       </c>
     </row>
-    <row r="266" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A266" s="19" t="s">
         <v>1207</v>
       </c>
@@ -25378,7 +25378,7 @@
         <v>3329.0410000000002</v>
       </c>
     </row>
-    <row r="279" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A279" s="19" t="s">
         <v>426</v>
       </c>
@@ -25422,7 +25422,7 @@
         <v>3334</v>
       </c>
     </row>
-    <row r="280" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A280" s="19" t="s">
         <v>1267</v>
       </c>
@@ -25463,7 +25463,7 @@
         <v>3334.0010000000002</v>
       </c>
     </row>
-    <row r="281" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A281" s="19" t="s">
         <v>1237</v>
       </c>
@@ -25504,7 +25504,7 @@
         <v>3334.0310000000004</v>
       </c>
     </row>
-    <row r="282" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A282" s="19" t="s">
         <v>1208</v>
       </c>
@@ -25545,7 +25545,7 @@
         <v>3334.0410000000002</v>
       </c>
     </row>
-    <row r="283" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A283" s="19" t="s">
         <v>404</v>
       </c>
@@ -25592,7 +25592,7 @@
         <v>3760</v>
       </c>
     </row>
-    <row r="284" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A284" s="19" t="s">
         <v>290</v>
       </c>
@@ -25636,7 +25636,7 @@
         <v>3760.0010000000002</v>
       </c>
     </row>
-    <row r="285" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A285" s="19" t="s">
         <v>995</v>
       </c>
@@ -25680,7 +25680,7 @@
         <v>3760.0310000000004</v>
       </c>
     </row>
-    <row r="286" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A286" s="19" t="s">
         <v>1210</v>
       </c>
@@ -25724,7 +25724,7 @@
         <v>3760.0410000000002</v>
       </c>
     </row>
-    <row r="287" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A287" s="19" t="s">
         <v>207</v>
       </c>
@@ -25771,7 +25771,7 @@
         <v>3761</v>
       </c>
     </row>
-    <row r="288" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A288" s="19" t="s">
         <v>291</v>
       </c>
@@ -25815,7 +25815,7 @@
         <v>3761.0010000000002</v>
       </c>
     </row>
-    <row r="289" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A289" s="19" t="s">
         <v>996</v>
       </c>
@@ -25859,7 +25859,7 @@
         <v>3761.0310000000004</v>
       </c>
     </row>
-    <row r="290" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A290" s="19" t="s">
         <v>1211</v>
       </c>
@@ -26699,7 +26699,7 @@
         <v>3349.0030000000002</v>
       </c>
     </row>
-    <row r="311" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A311" s="19" t="s">
         <v>881</v>
       </c>
@@ -26743,7 +26743,7 @@
         <v>3354</v>
       </c>
     </row>
-    <row r="312" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A312" s="19" t="s">
         <v>610</v>
       </c>
@@ -26784,7 +26784,7 @@
         <v>3354.0010000000002</v>
       </c>
     </row>
-    <row r="313" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A313" s="19" t="s">
         <v>1275</v>
       </c>
@@ -26825,7 +26825,7 @@
         <v>3354.002</v>
       </c>
     </row>
-    <row r="314" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A314" s="19" t="s">
         <v>385</v>
       </c>
@@ -27546,7 +27546,7 @@
         <v>3366.0030000000002</v>
       </c>
     </row>
-    <row r="331" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A331" s="19" t="s">
         <v>1</v>
       </c>
@@ -27590,7 +27590,7 @@
         <v>3371</v>
       </c>
     </row>
-    <row r="332" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A332" s="19" t="s">
         <v>622</v>
       </c>
@@ -27631,7 +27631,7 @@
         <v>3371.0010000000002</v>
       </c>
     </row>
-    <row r="333" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A333" s="19" t="s">
         <v>1301</v>
       </c>
@@ -27672,7 +27672,7 @@
         <v>3371.002</v>
       </c>
     </row>
-    <row r="334" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A334" s="19" t="s">
         <v>376</v>
       </c>
@@ -27880,7 +27880,7 @@
         <v>3376.0030000000002</v>
       </c>
     </row>
-    <row r="339" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A339" s="19" t="s">
         <v>880</v>
       </c>
@@ -27924,7 +27924,7 @@
         <v>3381</v>
       </c>
     </row>
-    <row r="340" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A340" s="19" t="s">
         <v>609</v>
       </c>
@@ -27965,7 +27965,7 @@
         <v>3381.0010000000002</v>
       </c>
     </row>
-    <row r="341" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A341" s="19" t="s">
         <v>1274</v>
       </c>
@@ -28006,7 +28006,7 @@
         <v>3381.002</v>
       </c>
     </row>
-    <row r="342" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A342" s="19" t="s">
         <v>384</v>
       </c>
@@ -28381,7 +28381,7 @@
         <v>3387.0030000000002</v>
       </c>
     </row>
-    <row r="351" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A351" s="19" t="s">
         <v>2361</v>
       </c>
@@ -28469,7 +28469,7 @@
         <v>3388</v>
       </c>
     </row>
-    <row r="353" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A353" s="19" t="s">
         <v>2362</v>
       </c>
@@ -28551,7 +28551,7 @@
         <v>3388.0010000000002</v>
       </c>
     </row>
-    <row r="355" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A355" s="19" t="s">
         <v>2363</v>
       </c>
@@ -28627,7 +28627,7 @@
         <v>3388.002</v>
       </c>
     </row>
-    <row r="357" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A357" s="19" t="s">
         <v>2364</v>
       </c>
@@ -28703,7 +28703,7 @@
         <v>3388.0030000000002</v>
       </c>
     </row>
-    <row r="359" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A359" s="19" t="s">
         <v>2365</v>
       </c>
@@ -28797,7 +28797,7 @@
         <v>3389</v>
       </c>
     </row>
-    <row r="361" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A361" s="19" t="s">
         <v>2366</v>
       </c>
@@ -28885,7 +28885,7 @@
         <v>3389.0010000000002</v>
       </c>
     </row>
-    <row r="363" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A363" s="19" t="s">
         <v>2367</v>
       </c>
@@ -28967,7 +28967,7 @@
         <v>3389.002</v>
       </c>
     </row>
-    <row r="365" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A365" s="19" t="s">
         <v>2368</v>
       </c>
@@ -32715,7 +32715,7 @@
         <v>3431.0920000000001</v>
       </c>
     </row>
-    <row r="454" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A454" s="19" t="s">
         <v>2373</v>
       </c>
@@ -32803,7 +32803,7 @@
         <v>3432</v>
       </c>
     </row>
-    <row r="456" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A456" s="19" t="s">
         <v>2374</v>
       </c>
@@ -32885,7 +32885,7 @@
         <v>3432.0010000000002</v>
       </c>
     </row>
-    <row r="458" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A458" s="19" t="s">
         <v>2375</v>
       </c>
@@ -32961,7 +32961,7 @@
         <v>3432.002</v>
       </c>
     </row>
-    <row r="460" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A460" s="19" t="s">
         <v>2376</v>
       </c>
@@ -33289,7 +33289,7 @@
         <v>3435.0920000000001</v>
       </c>
     </row>
-    <row r="468" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A468" s="19" t="s">
         <v>184</v>
       </c>
@@ -33336,7 +33336,7 @@
         <v>3440</v>
       </c>
     </row>
-    <row r="469" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A469" s="19" t="s">
         <v>185</v>
       </c>
@@ -33380,7 +33380,7 @@
         <v>3440.0010000000002</v>
       </c>
     </row>
-    <row r="470" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A470" s="19" t="s">
         <v>388</v>
       </c>
@@ -33424,7 +33424,7 @@
         <v>3440.002</v>
       </c>
     </row>
-    <row r="471" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A471" s="19" t="s">
         <v>389</v>
       </c>
@@ -33468,7 +33468,7 @@
         <v>3440.0030000000002</v>
       </c>
     </row>
-    <row r="472" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A472" s="19" t="s">
         <v>390</v>
       </c>
@@ -33515,7 +33515,7 @@
         <v>3444</v>
       </c>
     </row>
-    <row r="473" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A473" s="19" t="s">
         <v>391</v>
       </c>
@@ -33559,7 +33559,7 @@
         <v>3444.0010000000002</v>
       </c>
     </row>
-    <row r="474" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A474" s="19" t="s">
         <v>392</v>
       </c>
@@ -33603,7 +33603,7 @@
         <v>3444.002</v>
       </c>
     </row>
-    <row r="475" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A475" s="19" t="s">
         <v>393</v>
       </c>
@@ -33647,7 +33647,7 @@
         <v>3444.0030000000002</v>
       </c>
     </row>
-    <row r="476" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A476" s="19" t="s">
         <v>400</v>
       </c>
@@ -33694,7 +33694,7 @@
         <v>3835</v>
       </c>
     </row>
-    <row r="477" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A477" s="19" t="s">
         <v>401</v>
       </c>
@@ -33738,7 +33738,7 @@
         <v>3835.0010000000002</v>
       </c>
     </row>
-    <row r="478" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A478" s="19" t="s">
         <v>402</v>
       </c>
@@ -33782,7 +33782,7 @@
         <v>3835.002</v>
       </c>
     </row>
-    <row r="479" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A479" s="19" t="s">
         <v>403</v>
       </c>
@@ -33826,7 +33826,7 @@
         <v>3835.0030000000002</v>
       </c>
     </row>
-    <row r="480" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A480" s="19" t="s">
         <v>114</v>
       </c>
@@ -33873,7 +33873,7 @@
         <v>3445</v>
       </c>
     </row>
-    <row r="481" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A481" s="19" t="s">
         <v>115</v>
       </c>
@@ -33917,7 +33917,7 @@
         <v>3445.0010000000002</v>
       </c>
     </row>
-    <row r="482" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A482" s="19" t="s">
         <v>116</v>
       </c>
@@ -33958,7 +33958,7 @@
         <v>3445.002</v>
       </c>
     </row>
-    <row r="483" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A483" s="19" t="s">
         <v>117</v>
       </c>
@@ -34299,7 +34299,7 @@
         <v>3450.0010000000002</v>
       </c>
     </row>
-    <row r="491" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A491" s="19" t="s">
         <v>1479</v>
       </c>
@@ -34420,7 +34420,7 @@
         <v>3453.0010000000002</v>
       </c>
     </row>
-    <row r="494" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A494" s="19" t="s">
         <v>1481</v>
       </c>
@@ -34464,7 +34464,7 @@
         <v>3453.1</v>
       </c>
     </row>
-    <row r="495" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A495" s="19" t="s">
         <v>752</v>
       </c>
@@ -34508,7 +34508,7 @@
         <v>3457</v>
       </c>
     </row>
-    <row r="496" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A496" s="19" t="s">
         <v>815</v>
       </c>
@@ -34549,7 +34549,7 @@
         <v>3457.0010000000002</v>
       </c>
     </row>
-    <row r="497" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A497" s="19" t="s">
         <v>1482</v>
       </c>
@@ -34678,7 +34678,7 @@
         <v>3460.0010000000002</v>
       </c>
     </row>
-    <row r="500" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A500" s="19" t="s">
         <v>1486</v>
       </c>
@@ -34807,7 +34807,7 @@
         <v>3463.0010000000002</v>
       </c>
     </row>
-    <row r="503" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A503" s="19" t="s">
         <v>1487</v>
       </c>
@@ -34937,7 +34937,7 @@
         <v>3466.0010000000002</v>
       </c>
     </row>
-    <row r="506" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A506" s="19" t="s">
         <v>1483</v>
       </c>
@@ -35067,7 +35067,7 @@
         <v>3467.0010000000002</v>
       </c>
     </row>
-    <row r="509" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A509" s="19" t="s">
         <v>1484</v>
       </c>
@@ -35202,7 +35202,7 @@
         <v>3468.0010000000002</v>
       </c>
     </row>
-    <row r="512" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="512" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A512" s="19" t="s">
         <v>1485</v>
       </c>
@@ -35334,7 +35334,7 @@
         <v>3469.0010000000002</v>
       </c>
     </row>
-    <row r="515" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="515" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A515" s="19" t="s">
         <v>1488</v>
       </c>
@@ -35463,7 +35463,7 @@
         <v>3472.0010000000002</v>
       </c>
     </row>
-    <row r="518" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="518" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A518" s="19" t="s">
         <v>1489</v>
       </c>
@@ -35507,7 +35507,7 @@
         <v>3472.1</v>
       </c>
     </row>
-    <row r="519" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="519" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A519" s="19" t="s">
         <v>477</v>
       </c>
@@ -35551,7 +35551,7 @@
         <v>3473</v>
       </c>
     </row>
-    <row r="520" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="520" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A520" s="19" t="s">
         <v>143</v>
       </c>
@@ -35592,7 +35592,7 @@
         <v>3473.0010000000002</v>
       </c>
     </row>
-    <row r="521" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="521" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A521" s="19" t="s">
         <v>1490</v>
       </c>
@@ -35721,7 +35721,7 @@
         <v>3474.0010000000002</v>
       </c>
     </row>
-    <row r="524" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="524" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A524" s="19" t="s">
         <v>1491</v>
       </c>
@@ -35765,7 +35765,7 @@
         <v>3474.1</v>
       </c>
     </row>
-    <row r="525" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="525" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A525" s="19" t="s">
         <v>107</v>
       </c>
@@ -35812,7 +35812,7 @@
         <v>3475</v>
       </c>
     </row>
-    <row r="526" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="526" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A526" s="27" t="s">
         <v>841</v>
       </c>
@@ -35856,7 +35856,7 @@
         <v>3475.0010000000002</v>
       </c>
     </row>
-    <row r="527" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="527" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A527" s="19" t="s">
         <v>1492</v>
       </c>
@@ -35989,7 +35989,7 @@
         <v>3476.0010000000002</v>
       </c>
     </row>
-    <row r="530" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="530" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A530" s="19" t="s">
         <v>1493</v>
       </c>
@@ -36123,7 +36123,7 @@
         <v>3477.0010000000002</v>
       </c>
     </row>
-    <row r="533" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A533" s="19" t="s">
         <v>1494</v>
       </c>
@@ -36425,7 +36425,7 @@
         <v>3484.0010000000002</v>
       </c>
     </row>
-    <row r="540" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="540" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A540" s="19" t="s">
         <v>978</v>
       </c>
@@ -36469,7 +36469,7 @@
         <v>3488</v>
       </c>
     </row>
-    <row r="541" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="541" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A541" s="19" t="s">
         <v>351</v>
       </c>
@@ -36595,7 +36595,7 @@
         <v>3491.0010000000002</v>
       </c>
     </row>
-    <row r="544" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A544" s="19" t="s">
         <v>980</v>
       </c>
@@ -36640,7 +36640,7 @@
         <v>3492</v>
       </c>
     </row>
-    <row r="545" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="545" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A545" s="19" t="s">
         <v>125</v>
       </c>
@@ -37455,7 +37455,7 @@
         <v>3503.0010000000002</v>
       </c>
     </row>
-    <row r="564" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="564" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A564" s="19" t="s">
         <v>783</v>
       </c>
@@ -37499,7 +37499,7 @@
         <v>3504</v>
       </c>
     </row>
-    <row r="565" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="565" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A565" s="19" t="s">
         <v>11</v>
       </c>
@@ -37540,7 +37540,7 @@
         <v>3504.0010000000002</v>
       </c>
     </row>
-    <row r="566" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="566" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A566" s="19" t="s">
         <v>398</v>
       </c>
@@ -37587,7 +37587,7 @@
         <v>3505</v>
       </c>
     </row>
-    <row r="567" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="567" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A567" s="19" t="s">
         <v>399</v>
       </c>
@@ -37719,7 +37719,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="570" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="570" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A570" s="19" t="s">
         <v>74</v>
       </c>
@@ -37757,7 +37757,7 @@
         <v>3507</v>
       </c>
     </row>
-    <row r="571" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="571" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A571" s="19" t="s">
         <v>75</v>
       </c>
@@ -38858,7 +38858,7 @@
         <v>3523.0030000000002</v>
       </c>
     </row>
-    <row r="598" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="598" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A598" s="19" t="s">
         <v>630</v>
       </c>
@@ -38902,7 +38902,7 @@
         <v>3821</v>
       </c>
     </row>
-    <row r="599" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="599" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A599" s="19" t="s">
         <v>802</v>
       </c>
@@ -38943,7 +38943,7 @@
         <v>3821.0010000000002</v>
       </c>
     </row>
-    <row r="600" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="600" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A600" s="19" t="s">
         <v>474</v>
       </c>
@@ -38984,7 +38984,7 @@
         <v>3821.002</v>
       </c>
     </row>
-    <row r="601" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="601" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A601" s="19" t="s">
         <v>262</v>
       </c>
@@ -39192,7 +39192,7 @@
         <v>3833.0030000000002</v>
       </c>
     </row>
-    <row r="606" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="606" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A606" s="19" t="s">
         <v>394</v>
       </c>
@@ -39239,7 +39239,7 @@
         <v>3834</v>
       </c>
     </row>
-    <row r="607" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="607" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A607" s="19" t="s">
         <v>395</v>
       </c>
@@ -39283,7 +39283,7 @@
         <v>3834.0010000000002</v>
       </c>
     </row>
-    <row r="608" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="608" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A608" s="19" t="s">
         <v>396</v>
       </c>
@@ -39327,7 +39327,7 @@
         <v>3834.002</v>
       </c>
     </row>
-    <row r="609" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="609" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A609" s="19" t="s">
         <v>397</v>
       </c>
@@ -39371,7 +39371,7 @@
         <v>3834.0030000000002</v>
       </c>
     </row>
-    <row r="610" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="610" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A610" s="19" t="s">
         <v>118</v>
       </c>
@@ -39418,7 +39418,7 @@
         <v>3836</v>
       </c>
     </row>
-    <row r="611" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="611" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A611" s="19" t="s">
         <v>119</v>
       </c>
@@ -39459,7 +39459,7 @@
         <v>3836.0010000000002</v>
       </c>
     </row>
-    <row r="612" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="612" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A612" s="19" t="s">
         <v>120</v>
       </c>
@@ -39500,7 +39500,7 @@
         <v>3836.002</v>
       </c>
     </row>
-    <row r="613" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="613" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A613" s="19" t="s">
         <v>144</v>
       </c>
@@ -44097,7 +44097,7 @@
         <v>3580.0030000000002</v>
       </c>
     </row>
-    <row r="726" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="726" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A726" s="19" t="s">
         <v>440</v>
       </c>
@@ -44141,7 +44141,7 @@
         <v>3582</v>
       </c>
     </row>
-    <row r="727" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="727" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A727" s="19" t="s">
         <v>1293</v>
       </c>
@@ -44182,7 +44182,7 @@
         <v>3582.0010000000002</v>
       </c>
     </row>
-    <row r="728" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="728" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A728" s="19" t="s">
         <v>1082</v>
       </c>
@@ -44223,7 +44223,7 @@
         <v>3582.002</v>
       </c>
     </row>
-    <row r="729" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="729" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A729" s="19" t="s">
         <v>469</v>
       </c>
@@ -44425,7 +44425,7 @@
         <v>3825.0030000000002</v>
       </c>
     </row>
-    <row r="734" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="734" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A734" s="19" t="s">
         <v>2369</v>
       </c>
@@ -44513,7 +44513,7 @@
         <v>3826</v>
       </c>
     </row>
-    <row r="736" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="736" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A736" s="19" t="s">
         <v>2370</v>
       </c>
@@ -44595,7 +44595,7 @@
         <v>3826.0010000000002</v>
       </c>
     </row>
-    <row r="738" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="738" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A738" s="19" t="s">
         <v>2371</v>
       </c>
@@ -44671,7 +44671,7 @@
         <v>3826.002</v>
       </c>
     </row>
-    <row r="740" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="740" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A740" s="19" t="s">
         <v>2372</v>
       </c>
@@ -47207,7 +47207,7 @@
         <v>3618.0030000000002</v>
       </c>
     </row>
-    <row r="802" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="802" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A802" s="19" t="s">
         <v>2377</v>
       </c>
@@ -47295,7 +47295,7 @@
         <v>3619</v>
       </c>
     </row>
-    <row r="804" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="804" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A804" s="19" t="s">
         <v>2378</v>
       </c>
@@ -47377,7 +47377,7 @@
         <v>3619.0010000000002</v>
       </c>
     </row>
-    <row r="806" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="806" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A806" s="19" t="s">
         <v>2379</v>
       </c>
@@ -47453,7 +47453,7 @@
         <v>3619.002</v>
       </c>
     </row>
-    <row r="808" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="808" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A808" s="19" t="s">
         <v>2380</v>
       </c>
@@ -47696,7 +47696,7 @@
         <v>3620.0030000000002</v>
       </c>
     </row>
-    <row r="814" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="814" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A814" s="19" t="s">
         <v>926</v>
       </c>
@@ -47743,7 +47743,7 @@
         <v>3625</v>
       </c>
     </row>
-    <row r="815" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="815" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A815" s="19" t="s">
         <v>1029</v>
       </c>
@@ -47787,7 +47787,7 @@
         <v>3625.0010000000002</v>
       </c>
     </row>
-    <row r="816" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="816" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A816" s="19" t="s">
         <v>1077</v>
       </c>
@@ -47831,7 +47831,7 @@
         <v>3625.002</v>
       </c>
     </row>
-    <row r="817" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="817" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A817" s="19" t="s">
         <v>925</v>
       </c>
@@ -47875,7 +47875,7 @@
         <v>3625.0030000000002</v>
       </c>
     </row>
-    <row r="818" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="818" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A818" s="19" t="s">
         <v>450</v>
       </c>
@@ -47919,7 +47919,7 @@
         <v>3626</v>
       </c>
     </row>
-    <row r="819" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="819" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A819" s="19" t="s">
         <v>1102</v>
       </c>
@@ -47960,7 +47960,7 @@
         <v>3626.0010000000002</v>
       </c>
     </row>
-    <row r="820" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="820" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A820" s="19" t="s">
         <v>1129</v>
       </c>
@@ -48001,7 +48001,7 @@
         <v>3626.002</v>
       </c>
     </row>
-    <row r="821" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="821" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A821" s="19" t="s">
         <v>1260</v>
       </c>
@@ -48173,7 +48173,7 @@
         <v>3627.0030000000002</v>
       </c>
     </row>
-    <row r="826" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="826" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A826" s="19" t="s">
         <v>236</v>
       </c>
@@ -48218,7 +48218,7 @@
         <v>3628</v>
       </c>
     </row>
-    <row r="827" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="827" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A827" s="19" t="s">
         <v>1027</v>
       </c>
@@ -48260,7 +48260,7 @@
         <v>3628.0010000000002</v>
       </c>
     </row>
-    <row r="828" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="828" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A828" s="19" t="s">
         <v>1075</v>
       </c>
@@ -48302,7 +48302,7 @@
         <v>3628.002</v>
       </c>
     </row>
-    <row r="829" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="829" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A829" s="19" t="s">
         <v>992</v>
       </c>
@@ -48848,7 +48848,7 @@
         <v>3631.0030000000002</v>
       </c>
     </row>
-    <row r="842" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="842" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A842" s="19" t="s">
         <v>448</v>
       </c>
@@ -48895,7 +48895,7 @@
         <v>3632</v>
       </c>
     </row>
-    <row r="843" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="843" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A843" s="19" t="s">
         <v>818</v>
       </c>
@@ -48939,7 +48939,7 @@
         <v>3632.0010000000002</v>
       </c>
     </row>
-    <row r="844" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="844" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A844" s="19" t="s">
         <v>1079</v>
       </c>
@@ -48983,7 +48983,7 @@
         <v>3632.002</v>
       </c>
     </row>
-    <row r="845" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="845" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A845" s="19" t="s">
         <v>1122</v>
       </c>
@@ -49027,7 +49027,7 @@
         <v>3632.0030000000002</v>
       </c>
     </row>
-    <row r="846" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="846" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A846" s="19" t="s">
         <v>1429</v>
       </c>
@@ -49074,7 +49074,7 @@
         <v>3633</v>
       </c>
     </row>
-    <row r="847" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="847" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A847" s="19" t="s">
         <v>1431</v>
       </c>
@@ -49115,7 +49115,7 @@
         <v>3633.0010000000002</v>
       </c>
     </row>
-    <row r="848" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="848" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A848" s="19" t="s">
         <v>1432</v>
       </c>
@@ -49156,7 +49156,7 @@
         <v>3633.002</v>
       </c>
     </row>
-    <row r="849" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="849" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A849" s="19" t="s">
         <v>1433</v>
       </c>
@@ -49364,7 +49364,7 @@
         <v>3634.0030000000002</v>
       </c>
     </row>
-    <row r="854" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="854" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A854" s="19" t="s">
         <v>927</v>
       </c>
@@ -49408,7 +49408,7 @@
         <v>3639</v>
       </c>
     </row>
-    <row r="855" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="855" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A855" s="19" t="s">
         <v>1030</v>
       </c>
@@ -49449,7 +49449,7 @@
         <v>3639.0010000000002</v>
       </c>
     </row>
-    <row r="856" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="856" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A856" s="19" t="s">
         <v>1078</v>
       </c>
@@ -49490,7 +49490,7 @@
         <v>3639.002</v>
       </c>
     </row>
-    <row r="857" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="857" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A857" s="19" t="s">
         <v>1121</v>
       </c>
@@ -49531,7 +49531,7 @@
         <v>3639.0030000000002</v>
       </c>
     </row>
-    <row r="858" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="858" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A858" s="19" t="s">
         <v>449</v>
       </c>
@@ -49578,7 +49578,7 @@
         <v>3644</v>
       </c>
     </row>
-    <row r="859" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="859" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A859" s="19" t="s">
         <v>819</v>
       </c>
@@ -49622,7 +49622,7 @@
         <v>3644.0010000000002</v>
       </c>
     </row>
-    <row r="860" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="860" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A860" s="19" t="s">
         <v>1080</v>
       </c>
@@ -49666,7 +49666,7 @@
         <v>3644.002</v>
       </c>
     </row>
-    <row r="861" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="861" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A861" s="19" t="s">
         <v>1123</v>
       </c>
@@ -52987,7 +52987,7 @@
         <v>3681.0030000000002</v>
       </c>
     </row>
-    <row r="942" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="942" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A942" s="19" t="s">
         <v>820</v>
       </c>
@@ -53031,7 +53031,7 @@
         <v>3684</v>
       </c>
     </row>
-    <row r="943" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="943" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A943" s="19" t="s">
         <v>1296</v>
       </c>
@@ -53072,7 +53072,7 @@
         <v>3684.0010000000002</v>
       </c>
     </row>
-    <row r="944" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="944" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A944" s="19" t="s">
         <v>1217</v>
       </c>
@@ -53113,7 +53113,7 @@
         <v>3684.002</v>
       </c>
     </row>
-    <row r="945" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="945" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A945" s="19" t="s">
         <v>271</v>
       </c>
@@ -53679,7 +53679,7 @@
         <v>3829.0030000000002</v>
       </c>
     </row>
-    <row r="958" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="958" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A958" s="19" t="s">
         <v>1279</v>
       </c>
@@ -53723,7 +53723,7 @@
         <v>3830</v>
       </c>
     </row>
-    <row r="959" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="959" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A959" s="19" t="s">
         <v>697</v>
       </c>
@@ -53764,7 +53764,7 @@
         <v>3830.0010000000002</v>
       </c>
     </row>
-    <row r="960" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="960" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A960" s="19" t="s">
         <v>1149</v>
       </c>
@@ -53805,7 +53805,7 @@
         <v>3830.002</v>
       </c>
     </row>
-    <row r="961" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="961" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A961" s="19" t="s">
         <v>378</v>
       </c>
@@ -54342,7 +54342,7 @@
         <v>3694.0030000000002</v>
       </c>
     </row>
-    <row r="974" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="974" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A974" s="19" t="s">
         <v>1033</v>
       </c>
@@ -54392,7 +54392,7 @@
         <v>3694.14</v>
       </c>
     </row>
-    <row r="975" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="975" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A975" s="19" t="s">
         <v>1180</v>
       </c>
@@ -54433,7 +54433,7 @@
         <v>3694.1510000000003</v>
       </c>
     </row>
-    <row r="976" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="976" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A976" s="19" t="s">
         <v>1181</v>
       </c>
@@ -54471,7 +54471,7 @@
         <v>3694.1610000000001</v>
       </c>
     </row>
-    <row r="977" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="977" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A977" s="19" t="s">
         <v>1183</v>
       </c>
@@ -54509,7 +54509,7 @@
         <v>3694.1619999999998</v>
       </c>
     </row>
-    <row r="978" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="978" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A978" s="19" t="s">
         <v>204</v>
       </c>
@@ -54550,7 +54550,7 @@
         <v>3694.1710000000003</v>
       </c>
     </row>
-    <row r="979" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="979" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A979" s="19" t="s">
         <v>1036</v>
       </c>
@@ -54594,7 +54594,7 @@
         <v>3694.172</v>
       </c>
     </row>
-    <row r="980" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="980" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A980" s="19" t="s">
         <v>203</v>
       </c>
@@ -54717,7 +54717,7 @@
         <v>3699.0010000000002</v>
       </c>
     </row>
-    <row r="983" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="983" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A983" s="19" t="s">
         <v>920</v>
       </c>
@@ -54758,7 +54758,7 @@
         <v>3702</v>
       </c>
     </row>
-    <row r="984" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="984" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A984" s="19" t="s">
         <v>495</v>
       </c>
@@ -54790,7 +54790,7 @@
         <v>3702.0010000000002</v>
       </c>
     </row>
-    <row r="985" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="985" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A985" s="19" t="s">
         <v>1257</v>
       </c>
@@ -54822,7 +54822,7 @@
         <v>3702.002</v>
       </c>
     </row>
-    <row r="986" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="986" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A986" s="19" t="s">
         <v>22</v>
       </c>
@@ -54854,7 +54854,7 @@
         <v>3702.0030000000002</v>
       </c>
     </row>
-    <row r="987" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="987" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A987" s="19" t="s">
         <v>836</v>
       </c>
@@ -54898,7 +54898,7 @@
         <v>3707</v>
       </c>
     </row>
-    <row r="988" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="988" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A988" s="19" t="s">
         <v>496</v>
       </c>
@@ -54939,7 +54939,7 @@
         <v>3707.0010000000002</v>
       </c>
     </row>
-    <row r="989" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="989" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A989" s="19" t="s">
         <v>1099</v>
       </c>
@@ -54977,7 +54977,7 @@
         <v>3707.002</v>
       </c>
     </row>
-    <row r="990" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="990" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A990" s="19" t="s">
         <v>1101</v>
       </c>
@@ -55015,7 +55015,7 @@
         <v>3707.0030000000002</v>
       </c>
     </row>
-    <row r="991" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="991" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A991" s="19" t="s">
         <v>1281</v>
       </c>
@@ -55050,7 +55050,7 @@
         <v>3709</v>
       </c>
     </row>
-    <row r="992" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="992" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A992" s="19" t="s">
         <v>1138</v>
       </c>
@@ -55082,7 +55082,7 @@
         <v>3709.0010000000002</v>
       </c>
     </row>
-    <row r="993" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="993" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A993" s="19" t="s">
         <v>990</v>
       </c>
@@ -55114,7 +55114,7 @@
         <v>3709.002</v>
       </c>
     </row>
-    <row r="994" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="994" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A994" s="19" t="s">
         <v>380</v>
       </c>
@@ -55146,7 +55146,7 @@
         <v>3709.0030000000002</v>
       </c>
     </row>
-    <row r="995" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="995" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A995" s="19" t="s">
         <v>1268</v>
       </c>
@@ -55190,7 +55190,7 @@
         <v>3714</v>
       </c>
     </row>
-    <row r="996" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="996" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A996" s="19" t="s">
         <v>72</v>
       </c>
@@ -55231,7 +55231,7 @@
         <v>3714.0010000000002</v>
       </c>
     </row>
-    <row r="997" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="997" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A997" s="19" t="s">
         <v>1255</v>
       </c>
@@ -55272,7 +55272,7 @@
         <v>3714.002</v>
       </c>
     </row>
-    <row r="998" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="998" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A998" s="19" t="s">
         <v>381</v>
       </c>
@@ -55398,7 +55398,7 @@
         <v>3716.0010000000002</v>
       </c>
     </row>
-    <row r="1001" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1001" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1001" s="19" t="s">
         <v>837</v>
       </c>
@@ -55442,7 +55442,7 @@
         <v>3719</v>
       </c>
     </row>
-    <row r="1002" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1002" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1002" s="19" t="s">
         <v>497</v>
       </c>
@@ -55617,7 +55617,7 @@
         <v>3721.0010000000002</v>
       </c>
     </row>
-    <row r="1007" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1007" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1007" s="19" t="s">
         <v>223</v>
       </c>
@@ -55661,7 +55661,7 @@
         <v>3813</v>
       </c>
     </row>
-    <row r="1008" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1008" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1008" s="19" t="s">
         <v>1072</v>
       </c>
@@ -55702,7 +55702,7 @@
         <v>3813.0010000000002</v>
       </c>
     </row>
-    <row r="1009" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1009" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1009" s="19" t="s">
         <v>54</v>
       </c>
@@ -55747,7 +55747,7 @@
         <v>3814</v>
       </c>
     </row>
-    <row r="1010" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1010" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1010" s="19" t="s">
         <v>542</v>
       </c>
@@ -55788,7 +55788,7 @@
         <v>3814.0010000000002</v>
       </c>
     </row>
-    <row r="1011" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1011" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1011" s="19" t="s">
         <v>1463</v>
       </c>
@@ -55830,7 +55830,7 @@
         <v>3814.18</v>
       </c>
     </row>
-    <row r="1012" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1012" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1012" s="19" t="s">
         <v>1467</v>
       </c>
@@ -55871,7 +55871,7 @@
         <v>3814.181</v>
       </c>
     </row>
-    <row r="1013" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1013" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1013" s="19" t="s">
         <v>58</v>
       </c>
@@ -55916,7 +55916,7 @@
         <v>3740</v>
       </c>
     </row>
-    <row r="1014" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1014" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1014" s="19" t="s">
         <v>1038</v>
       </c>
@@ -55957,7 +55957,7 @@
         <v>3740.0010000000002</v>
       </c>
     </row>
-    <row r="1015" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1015" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1015" s="19" t="s">
         <v>1465</v>
       </c>
@@ -55999,7 +55999,7 @@
         <v>3740.18</v>
       </c>
     </row>
-    <row r="1016" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1016" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1016" s="19" t="s">
         <v>1468</v>
       </c>
@@ -56040,7 +56040,7 @@
         <v>3740.181</v>
       </c>
     </row>
-    <row r="1017" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1017" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1017" s="19" t="s">
         <v>55</v>
       </c>
@@ -56085,7 +56085,7 @@
         <v>3724</v>
       </c>
     </row>
-    <row r="1018" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1018" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1018" s="19" t="s">
         <v>577</v>
       </c>
@@ -56381,7 +56381,7 @@
         <v>3727.0010000000002</v>
       </c>
     </row>
-    <row r="1025" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1025" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1025" s="19" t="s">
         <v>217</v>
       </c>
@@ -56428,7 +56428,7 @@
         <v>3730</v>
       </c>
     </row>
-    <row r="1026" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1026" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1026" s="19" t="s">
         <v>108</v>
       </c>
@@ -56469,7 +56469,7 @@
         <v>3730.0010000000002</v>
       </c>
     </row>
-    <row r="1027" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1027" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1027" s="19" t="s">
         <v>49</v>
       </c>
@@ -56516,7 +56516,7 @@
         <v>3731</v>
       </c>
     </row>
-    <row r="1028" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1028" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1028" s="19" t="s">
         <v>109</v>
       </c>
@@ -56557,7 +56557,7 @@
         <v>3731.0010000000002</v>
       </c>
     </row>
-    <row r="1029" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1029" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1029" s="19" t="s">
         <v>46</v>
       </c>
@@ -56604,7 +56604,7 @@
         <v>3732</v>
       </c>
     </row>
-    <row r="1030" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1030" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1030" s="19" t="s">
         <v>47</v>
       </c>
@@ -56646,7 +56646,7 @@
         <v>3732.0010000000002</v>
       </c>
     </row>
-    <row r="1031" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1031" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1031" s="19" t="s">
         <v>1435</v>
       </c>
@@ -56686,7 +56686,7 @@
         <v>3733</v>
       </c>
     </row>
-    <row r="1032" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1032" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1032" s="19" t="s">
         <v>1436</v>
       </c>
@@ -56718,7 +56718,7 @@
         <v>3733.0010000000002</v>
       </c>
     </row>
-    <row r="1033" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1033" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1033" s="19" t="s">
         <v>56</v>
       </c>
@@ -56762,7 +56762,7 @@
         <v>3734</v>
       </c>
     </row>
-    <row r="1034" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1034" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1034" s="19" t="s">
         <v>578</v>
       </c>
@@ -57298,7 +57298,7 @@
         <v>3752.0030000000002</v>
       </c>
     </row>
-    <row r="1047" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1047" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1047" s="19" t="s">
         <v>1449</v>
       </c>
@@ -59036,7 +59036,7 @@
         <v>3788.0030000000002</v>
       </c>
     </row>
-    <row r="1088" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1088" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1088" s="19" t="s">
         <v>210</v>
       </c>
@@ -59083,7 +59083,7 @@
         <v>3789</v>
       </c>
     </row>
-    <row r="1089" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1089" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1089" s="19" t="s">
         <v>88</v>
       </c>
@@ -59127,7 +59127,7 @@
         <v>3789.0010000000002</v>
       </c>
     </row>
-    <row r="1090" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1090" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1090" s="19" t="s">
         <v>278</v>
       </c>
@@ -59174,7 +59174,7 @@
         <v>3789.002</v>
       </c>
     </row>
-    <row r="1091" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1091" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1091" s="19" t="s">
         <v>284</v>
       </c>
@@ -59221,7 +59221,7 @@
         <v>3789.0030000000002</v>
       </c>
     </row>
-    <row r="1092" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1092" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1092" s="19" t="s">
         <v>211</v>
       </c>
@@ -59268,7 +59268,7 @@
         <v>3790</v>
       </c>
     </row>
-    <row r="1093" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1093" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1093" s="19" t="s">
         <v>89</v>
       </c>
@@ -59312,7 +59312,7 @@
         <v>3790.0010000000002</v>
       </c>
     </row>
-    <row r="1094" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1094" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1094" s="19" t="s">
         <v>279</v>
       </c>
@@ -59359,7 +59359,7 @@
         <v>3790.002</v>
       </c>
     </row>
-    <row r="1095" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1095" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1095" s="19" t="s">
         <v>285</v>
       </c>
@@ -59406,7 +59406,7 @@
         <v>3790.0030000000002</v>
       </c>
     </row>
-    <row r="1096" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1096" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1096" s="19" t="s">
         <v>212</v>
       </c>
@@ -59453,7 +59453,7 @@
         <v>3791</v>
       </c>
     </row>
-    <row r="1097" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1097" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1097" s="19" t="s">
         <v>214</v>
       </c>
@@ -59494,7 +59494,7 @@
         <v>3791.0010000000002</v>
       </c>
     </row>
-    <row r="1098" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1098" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1098" s="19" t="s">
         <v>215</v>
       </c>
@@ -59535,7 +59535,7 @@
         <v>3791.002</v>
       </c>
     </row>
-    <row r="1099" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1099" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1099" s="19" t="s">
         <v>216</v>
       </c>
@@ -59576,7 +59576,7 @@
         <v>3791.0030000000002</v>
       </c>
     </row>
-    <row r="1100" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1100" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1100" s="19" t="s">
         <v>162</v>
       </c>
@@ -59615,7 +59615,7 @@
         <v>3792</v>
       </c>
     </row>
-    <row r="1101" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1101" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1101" s="19" t="s">
         <v>615</v>
       </c>
@@ -59650,7 +59650,7 @@
         <v>3792.0010000000002</v>
       </c>
     </row>
-    <row r="1102" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1102" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1102" s="19" t="s">
         <v>1312</v>
       </c>
@@ -59697,7 +59697,7 @@
         <v>3793</v>
       </c>
     </row>
-    <row r="1103" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1103" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1103" s="19" t="s">
         <v>1313</v>
       </c>
@@ -59738,7 +59738,7 @@
         <v>3793.0010000000002</v>
       </c>
     </row>
-    <row r="1104" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1104" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1104" s="19" t="s">
         <v>1314</v>
       </c>
@@ -59779,7 +59779,7 @@
         <v>3793.002</v>
       </c>
     </row>
-    <row r="1105" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1105" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1105" s="19" t="s">
         <v>1315</v>
       </c>
@@ -60401,7 +60401,7 @@
         <v>3804.0010000000002</v>
       </c>
     </row>
-    <row r="1120" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1120" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1120" s="19" t="s">
         <v>693</v>
       </c>
@@ -60445,7 +60445,7 @@
         <v>3807</v>
       </c>
     </row>
-    <row r="1121" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1121" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1121" s="19" t="s">
         <v>612</v>
       </c>
@@ -60486,7 +60486,7 @@
         <v>3807.0010000000002</v>
       </c>
     </row>
-    <row r="1122" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1122" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1122" s="19" t="s">
         <v>110</v>
       </c>
@@ -60533,7 +60533,7 @@
         <v>3810</v>
       </c>
     </row>
-    <row r="1123" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1123" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1123" s="19" t="s">
         <v>112</v>
       </c>
@@ -60574,7 +60574,7 @@
         <v>3810.0010000000002</v>
       </c>
     </row>
-    <row r="1124" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1124" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1124" s="19" t="s">
         <v>1238</v>
       </c>
@@ -60618,7 +60618,7 @@
         <v>3810.002</v>
       </c>
     </row>
-    <row r="1125" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1125" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1125" s="19" t="s">
         <v>1240</v>
       </c>
@@ -60662,7 +60662,7 @@
         <v>3810.0030000000002</v>
       </c>
     </row>
-    <row r="1126" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1126" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1126" s="19" t="s">
         <v>111</v>
       </c>
@@ -60709,7 +60709,7 @@
         <v>3811</v>
       </c>
     </row>
-    <row r="1127" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1127" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1127" s="19" t="s">
         <v>113</v>
       </c>
@@ -60750,7 +60750,7 @@
         <v>3811.0010000000002</v>
       </c>
     </row>
-    <row r="1128" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1128" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1128" s="19" t="s">
         <v>1239</v>
       </c>
@@ -60794,7 +60794,7 @@
         <v>3811.002</v>
       </c>
     </row>
-    <row r="1129" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1129" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1129" s="19" t="s">
         <v>1241</v>
       </c>
@@ -60838,7 +60838,7 @@
         <v>3811.0030000000002</v>
       </c>
     </row>
-    <row r="1130" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1130" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1130" s="19" t="s">
         <v>1332</v>
       </c>
@@ -60879,7 +60879,7 @@
         <v>3812</v>
       </c>
     </row>
-    <row r="1131" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1131" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1131" s="19" t="s">
         <v>1333</v>
       </c>
@@ -60915,7 +60915,7 @@
         <v>3812.0010000000002</v>
       </c>
     </row>
-    <row r="1132" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1132" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1132" s="19" t="s">
         <v>586</v>
       </c>
@@ -60959,7 +60959,7 @@
         <v>3816</v>
       </c>
     </row>
-    <row r="1133" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1133" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1133" s="19" t="s">
         <v>858</v>
       </c>
@@ -61000,7 +61000,7 @@
         <v>3816.0010000000002</v>
       </c>
     </row>
-    <row r="1134" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1134" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1134" s="19" t="s">
         <v>1040</v>
       </c>
@@ -61041,7 +61041,7 @@
         <v>3816.002</v>
       </c>
     </row>
-    <row r="1135" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1135" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1135" s="19" t="s">
         <v>352</v>
       </c>
@@ -61289,7 +61289,7 @@
         <v>4293</v>
       </c>
     </row>
-    <row r="1142" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1142" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1142" s="19" t="s">
         <v>525</v>
       </c>
@@ -61324,7 +61324,7 @@
         <v>4294</v>
       </c>
     </row>
-    <row r="1143" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1143" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1143" s="19" t="s">
         <v>145</v>
       </c>
@@ -61362,7 +61362,7 @@
         <v>4297</v>
       </c>
     </row>
-    <row r="1144" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1144" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1144" s="19" t="s">
         <v>146</v>
       </c>
@@ -61400,7 +61400,7 @@
         <v>4298</v>
       </c>
     </row>
-    <row r="1145" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1145" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1145" s="19" t="s">
         <v>80</v>
       </c>
@@ -61476,7 +61476,7 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="1147" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1147" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1147" s="19" t="s">
         <v>147</v>
       </c>
@@ -61549,7 +61549,7 @@
         <v>4311</v>
       </c>
     </row>
-    <row r="1149" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1149" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1149" s="19" t="s">
         <v>1421</v>
       </c>
@@ -62009,7 +62009,7 @@
         <v>4356</v>
       </c>
     </row>
-    <row r="1162" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1162" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1162" s="19" t="s">
         <v>1459</v>
       </c>
@@ -62425,7 +62425,7 @@
         <v>4385</v>
       </c>
     </row>
-    <row r="1174" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1174" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1174" s="19" t="s">
         <v>1472</v>
       </c>
@@ -62457,7 +62457,7 @@
         <v>4385.26</v>
       </c>
     </row>
-    <row r="1175" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1175" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1175" s="19" t="s">
         <v>757</v>
       </c>
@@ -62947,7 +62947,7 @@
         <v>4401</v>
       </c>
     </row>
-    <row r="1189" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1189" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1189" s="19" t="s">
         <v>68</v>
       </c>
@@ -63052,7 +63052,7 @@
         <v>4404</v>
       </c>
     </row>
-    <row r="1192" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1192" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1192" s="19" t="s">
         <v>616</v>
       </c>
@@ -63300,7 +63300,7 @@
         <v>4409</v>
       </c>
     </row>
-    <row r="1199" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1199" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1199" s="19" t="s">
         <v>945</v>
       </c>
@@ -64465,7 +64465,7 @@
         <v>4424.0050000000001</v>
       </c>
     </row>
-    <row r="1234" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1234" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1234" s="19" t="s">
         <v>1162</v>
       </c>
@@ -64491,7 +64491,7 @@
         <v>1229</v>
       </c>
       <c r="J1234" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="Z1234" t="s">
         <v>2784</v>
@@ -64500,7 +64500,7 @@
         <v>4425</v>
       </c>
     </row>
-    <row r="1235" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1235" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1235" s="19" t="s">
         <v>606</v>
       </c>
@@ -64526,13 +64526,13 @@
         <v>1230</v>
       </c>
       <c r="J1235" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="AA1235">
         <v>4425.0039999999999</v>
       </c>
     </row>
-    <row r="1236" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1236" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1236" s="19" t="s">
         <v>591</v>
       </c>
@@ -64558,13 +64558,13 @@
         <v>1231</v>
       </c>
       <c r="J1236" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="AA1236">
         <v>4425.0050000000001</v>
       </c>
     </row>
-    <row r="1237" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1237" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1237" s="19" t="s">
         <v>1163</v>
       </c>
@@ -64590,7 +64590,7 @@
         <v>1232</v>
       </c>
       <c r="J1237" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="Z1237" t="s">
         <v>2785</v>
@@ -64599,7 +64599,7 @@
         <v>4426</v>
       </c>
     </row>
-    <row r="1238" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1238" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1238" s="19" t="s">
         <v>706</v>
       </c>
@@ -64625,13 +64625,13 @@
         <v>1233</v>
       </c>
       <c r="J1238" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="AA1238">
         <v>4426.0039999999999</v>
       </c>
     </row>
-    <row r="1239" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1239" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1239" s="19" t="s">
         <v>592</v>
       </c>
@@ -64657,13 +64657,13 @@
         <v>1234</v>
       </c>
       <c r="J1239" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="AA1239">
         <v>4426.0050000000001</v>
       </c>
     </row>
-    <row r="1240" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1240" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1240" s="19" t="s">
         <v>1164</v>
       </c>
@@ -64689,7 +64689,7 @@
         <v>1235</v>
       </c>
       <c r="J1240" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="Z1240" t="s">
         <v>2786</v>
@@ -64698,7 +64698,7 @@
         <v>4427</v>
       </c>
     </row>
-    <row r="1241" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1241" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1241" s="19" t="s">
         <v>707</v>
       </c>
@@ -64724,13 +64724,13 @@
         <v>1236</v>
       </c>
       <c r="J1241" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="AA1241">
         <v>4427.0039999999999</v>
       </c>
     </row>
-    <row r="1242" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1242" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1242" s="19" t="s">
         <v>593</v>
       </c>
@@ -64756,13 +64756,13 @@
         <v>1237</v>
       </c>
       <c r="J1242" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="AA1242">
         <v>4427.0050000000001</v>
       </c>
     </row>
-    <row r="1243" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1243" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1243" s="19" t="s">
         <v>1263</v>
       </c>
@@ -64788,7 +64788,7 @@
         <v>1238</v>
       </c>
       <c r="J1243" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="Z1243" t="s">
         <v>2787</v>
@@ -64797,7 +64797,7 @@
         <v>4428</v>
       </c>
     </row>
-    <row r="1244" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1244" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1244" s="19" t="s">
         <v>472</v>
       </c>
@@ -64823,13 +64823,13 @@
         <v>1239</v>
       </c>
       <c r="J1244" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="AA1244">
         <v>4428.0039999999999</v>
       </c>
     </row>
-    <row r="1245" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1245" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1245" s="19" t="s">
         <v>371</v>
       </c>
@@ -64855,13 +64855,13 @@
         <v>1240</v>
       </c>
       <c r="J1245" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="AA1245">
         <v>4428.0050000000001</v>
       </c>
     </row>
-    <row r="1246" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1246" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1246" s="19" t="s">
         <v>1264</v>
       </c>
@@ -64887,7 +64887,7 @@
         <v>1241</v>
       </c>
       <c r="J1246" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="W1246" s="5"/>
       <c r="Z1246" t="s">
@@ -64897,7 +64897,7 @@
         <v>4429</v>
       </c>
     </row>
-    <row r="1247" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1247" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1247" s="19" t="s">
         <v>708</v>
       </c>
@@ -64923,14 +64923,14 @@
         <v>1242</v>
       </c>
       <c r="J1247" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="W1247" s="5"/>
       <c r="AA1247">
         <v>4429.0039999999999</v>
       </c>
     </row>
-    <row r="1248" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1248" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1248" s="19" t="s">
         <v>157</v>
       </c>
@@ -64956,14 +64956,14 @@
         <v>1243</v>
       </c>
       <c r="J1248" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="W1248" s="5"/>
       <c r="AA1248">
         <v>4429.0050000000001</v>
       </c>
     </row>
-    <row r="1249" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1249" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1249" s="19" t="s">
         <v>1189</v>
       </c>
@@ -64989,7 +64989,7 @@
         <v>1244</v>
       </c>
       <c r="J1249" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="U1249" t="s">
         <v>1452</v>
@@ -65007,7 +65007,7 @@
         <v>4429.2700000000004</v>
       </c>
     </row>
-    <row r="1250" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1250" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1250" s="19" t="s">
         <v>1192</v>
       </c>
@@ -65033,7 +65033,7 @@
         <v>1245</v>
       </c>
       <c r="J1250" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="U1250" t="s">
         <v>1452</v>
@@ -65048,7 +65048,7 @@
         <v>4429.2740000000003</v>
       </c>
     </row>
-    <row r="1251" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1251" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1251" s="19" t="s">
         <v>775</v>
       </c>
@@ -65074,7 +65074,7 @@
         <v>1246</v>
       </c>
       <c r="J1251" s="11" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="U1251" t="s">
         <v>1452</v>
@@ -65089,7 +65089,7 @@
         <v>4429.2750000000005</v>
       </c>
     </row>
-    <row r="1252" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1252" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1252" s="19" t="s">
         <v>1553</v>
       </c>
@@ -65133,7 +65133,7 @@
         <v>4429.28</v>
       </c>
     </row>
-    <row r="1253" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1253" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1253" s="19" t="s">
         <v>1555</v>
       </c>
@@ -65174,7 +65174,7 @@
         <v>4429.2839999999997</v>
       </c>
     </row>
-    <row r="1254" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1254" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1254" s="19" t="s">
         <v>1554</v>
       </c>
@@ -65218,7 +65218,7 @@
         <v>4429.2849999999999</v>
       </c>
     </row>
-    <row r="1255" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1255" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1255" s="19" t="s">
         <v>1265</v>
       </c>
@@ -65253,7 +65253,7 @@
         <v>4430</v>
       </c>
     </row>
-    <row r="1256" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1256" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1256" s="19" t="s">
         <v>709</v>
       </c>
@@ -65285,7 +65285,7 @@
         <v>4430.0039999999999</v>
       </c>
     </row>
-    <row r="1257" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1257" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1257" s="19" t="s">
         <v>158</v>
       </c>
@@ -65317,7 +65317,7 @@
         <v>4430.0050000000001</v>
       </c>
     </row>
-    <row r="1258" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1258" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1258" s="19" t="s">
         <v>1266</v>
       </c>
@@ -65353,7 +65353,7 @@
         <v>4431</v>
       </c>
     </row>
-    <row r="1259" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1259" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1259" s="19" t="s">
         <v>710</v>
       </c>
@@ -65386,7 +65386,7 @@
         <v>4431.0039999999999</v>
       </c>
     </row>
-    <row r="1260" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1260" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1260" s="19" t="s">
         <v>354</v>
       </c>
@@ -65419,7 +65419,7 @@
         <v>4431.0050000000001</v>
       </c>
     </row>
-    <row r="1261" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1261" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1261" s="19" t="s">
         <v>1190</v>
       </c>
@@ -65460,7 +65460,7 @@
         <v>4431.2700000000004</v>
       </c>
     </row>
-    <row r="1262" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1262" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1262" s="19" t="s">
         <v>1193</v>
       </c>
@@ -65498,7 +65498,7 @@
         <v>4431.2740000000003</v>
       </c>
     </row>
-    <row r="1263" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1263" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1263" s="19" t="s">
         <v>776</v>
       </c>
@@ -65536,7 +65536,7 @@
         <v>4431.2750000000005</v>
       </c>
     </row>
-    <row r="1264" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1264" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1264" s="19" t="s">
         <v>1048</v>
       </c>
@@ -65572,7 +65572,7 @@
         <v>4432</v>
       </c>
     </row>
-    <row r="1265" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1265" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1265" s="19" t="s">
         <v>711</v>
       </c>
@@ -65605,7 +65605,7 @@
         <v>4432.0039999999999</v>
       </c>
     </row>
-    <row r="1266" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1266" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1266" s="19" t="s">
         <v>590</v>
       </c>
@@ -65638,7 +65638,7 @@
         <v>4432.0050000000001</v>
       </c>
     </row>
-    <row r="1267" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1267" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1267" s="19" t="s">
         <v>1191</v>
       </c>
@@ -65679,7 +65679,7 @@
         <v>4432.2700000000004</v>
       </c>
     </row>
-    <row r="1268" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1268" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1268" s="19" t="s">
         <v>774</v>
       </c>
@@ -65720,7 +65720,7 @@
         <v>4432.2740000000003</v>
       </c>
     </row>
-    <row r="1269" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1269" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1269" s="19" t="s">
         <v>777</v>
       </c>
@@ -65761,7 +65761,7 @@
         <v>4432.2750000000005</v>
       </c>
     </row>
-    <row r="1270" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1270" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1270" s="19" t="s">
         <v>1049</v>
       </c>
@@ -65796,7 +65796,7 @@
         <v>4433</v>
       </c>
     </row>
-    <row r="1271" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1271" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1271" s="19" t="s">
         <v>712</v>
       </c>
@@ -65829,7 +65829,7 @@
         <v>4433.0039999999999</v>
       </c>
     </row>
-    <row r="1272" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1272" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1272" s="19" t="s">
         <v>372</v>
       </c>
@@ -65861,7 +65861,7 @@
         <v>4433.0050000000001</v>
       </c>
     </row>
-    <row r="1273" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1273" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1273" s="19" t="s">
         <v>1050</v>
       </c>
@@ -65896,7 +65896,7 @@
         <v>4434</v>
       </c>
     </row>
-    <row r="1274" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1274" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1274" s="19" t="s">
         <v>942</v>
       </c>
@@ -65928,7 +65928,7 @@
         <v>4434.0039999999999</v>
       </c>
     </row>
-    <row r="1275" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1275" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1275" s="19" t="s">
         <v>598</v>
       </c>
@@ -67000,7 +67000,7 @@
         <v>4450.32</v>
       </c>
     </row>
-    <row r="1306" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1306" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1306" s="19" t="s">
         <v>1437</v>
       </c>
@@ -67038,7 +67038,7 @@
         <v>4451</v>
       </c>
     </row>
-    <row r="1307" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1307" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1307" s="19" t="s">
         <v>1438</v>
       </c>
@@ -67070,7 +67070,7 @@
         <v>4451.3</v>
       </c>
     </row>
-    <row r="1308" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1308" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1308" s="19" t="s">
         <v>1439</v>
       </c>
@@ -67102,7 +67102,7 @@
         <v>4451.3100000000004</v>
       </c>
     </row>
-    <row r="1309" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1309" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1309" s="19" t="s">
         <v>1446</v>
       </c>
@@ -67134,7 +67134,7 @@
         <v>4451.32</v>
       </c>
     </row>
-    <row r="1310" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1310" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1310" s="19" t="s">
         <v>178</v>
       </c>
@@ -67172,7 +67172,7 @@
         <v>4452</v>
       </c>
     </row>
-    <row r="1311" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1311" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1311" s="19" t="s">
         <v>179</v>
       </c>
@@ -67210,7 +67210,7 @@
         <v>4453</v>
       </c>
     </row>
-    <row r="1312" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1312" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1312" s="19" t="s">
         <v>180</v>
       </c>
@@ -67359,7 +67359,7 @@
         <v>4457</v>
       </c>
     </row>
-    <row r="1316" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1316" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1316" s="19" t="s">
         <v>645</v>
       </c>
@@ -67394,7 +67394,7 @@
         <v>4458</v>
       </c>
     </row>
-    <row r="1317" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1317" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1317" s="19" t="s">
         <v>646</v>
       </c>
@@ -67429,7 +67429,7 @@
         <v>4459</v>
       </c>
     </row>
-    <row r="1318" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1318" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1318" s="19" t="s">
         <v>647</v>
       </c>
@@ -67464,7 +67464,7 @@
         <v>4460</v>
       </c>
     </row>
-    <row r="1319" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1319" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1319" s="19" t="s">
         <v>48</v>
       </c>
@@ -67508,7 +67508,7 @@
         <v>4461</v>
       </c>
     </row>
-    <row r="1320" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1320" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1320" s="19" t="s">
         <v>1252</v>
       </c>
@@ -67552,7 +67552,7 @@
         <v>4462</v>
       </c>
     </row>
-    <row r="1321" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1321" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1321" s="19" t="s">
         <v>1165</v>
       </c>
@@ -67891,7 +67891,7 @@
         <v>4465.38</v>
       </c>
     </row>
-    <row r="1331" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1331" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1331" s="19" t="s">
         <v>2334</v>
       </c>
@@ -67929,7 +67929,7 @@
         <v>3487</v>
       </c>
     </row>
-    <row r="1332" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1332" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1332" s="19" t="s">
         <v>1242</v>
       </c>
@@ -67967,7 +67967,7 @@
         <v>4466</v>
       </c>
     </row>
-    <row r="1333" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1333" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1333" s="19" t="s">
         <v>1243</v>
       </c>
@@ -68005,7 +68005,7 @@
         <v>4467</v>
       </c>
     </row>
-    <row r="1334" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1334" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1334" s="19" t="s">
         <v>1244</v>
       </c>
@@ -68043,7 +68043,7 @@
         <v>4468</v>
       </c>
     </row>
-    <row r="1335" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1335" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1335" s="19" t="s">
         <v>37</v>
       </c>
@@ -68081,7 +68081,7 @@
         <v>4469</v>
       </c>
     </row>
-    <row r="1336" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1336" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1336" s="19" t="s">
         <v>38</v>
       </c>
@@ -68119,7 +68119,7 @@
         <v>4470</v>
       </c>
     </row>
-    <row r="1337" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1337" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1337" s="19" t="s">
         <v>39</v>
       </c>
@@ -68926,7 +68926,7 @@
         <v>4491</v>
       </c>
     </row>
-    <row r="1358" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1358" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1358" s="19" t="s">
         <v>1374</v>
       </c>
@@ -69104,7 +69104,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1363" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1363" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1363" s="19" t="s">
         <v>1470</v>
       </c>
@@ -69293,7 +69293,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1369" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1369" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1369" s="19" t="s">
         <v>1462</v>
       </c>
@@ -70330,7 +70330,7 @@
         <v>22077</v>
       </c>
     </row>
-    <row r="1400" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1400" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1400" s="19" t="s">
         <v>259</v>
       </c>
@@ -70391,7 +70391,7 @@
         <v>22078</v>
       </c>
     </row>
-    <row r="1402" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1402" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1402" s="19" t="s">
         <v>260</v>
       </c>
@@ -70484,7 +70484,7 @@
         <v>22081</v>
       </c>
     </row>
-    <row r="1405" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1405" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1405" s="19" t="s">
         <v>751</v>
       </c>
@@ -70545,7 +70545,7 @@
         <v>22082</v>
       </c>
     </row>
-    <row r="1407" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1407" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1407" s="19" t="s">
         <v>753</v>
       </c>
@@ -71528,7 +71528,7 @@
         <v>22927</v>
       </c>
     </row>
-    <row r="1436" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1436" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1436" s="19" t="s">
         <v>1213</v>
       </c>
@@ -71566,7 +71566,7 @@
         <v>22928</v>
       </c>
     </row>
-    <row r="1437" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1437" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1437" s="19" t="s">
         <v>1214</v>
       </c>
@@ -71766,7 +71766,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1444" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1444" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1444" s="19" t="s">
         <v>1466</v>
       </c>
@@ -71872,7 +71872,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1448" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1448" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1448" s="19" t="s">
         <v>657</v>
       </c>
@@ -71924,7 +71924,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1450" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1450" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1450" s="19" t="s">
         <v>902</v>
       </c>
@@ -72054,7 +72054,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1455" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1455" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1455" s="19" t="s">
         <v>675</v>
       </c>
@@ -72080,7 +72080,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1456" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1456" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1456" s="19" t="s">
         <v>677</v>
       </c>
@@ -72106,7 +72106,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1457" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1457" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1457" s="19" t="s">
         <v>2248</v>
       </c>
@@ -72132,7 +72132,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1458" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1458" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1458" s="19" t="s">
         <v>213</v>
       </c>
@@ -72184,7 +72184,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1460" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1460" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1460" s="19" t="s">
         <v>672</v>
       </c>
@@ -72210,7 +72210,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1461" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1461" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1461" s="19" t="s">
         <v>676</v>
       </c>
@@ -72236,7 +72236,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1462" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1462" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1462" s="19" t="s">
         <v>1430</v>
       </c>
@@ -72288,7 +72288,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1464" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1464" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1464" s="19" t="s">
         <v>295</v>
       </c>
@@ -72314,7 +72314,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1465" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1465" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1465" s="19" t="s">
         <v>296</v>
       </c>
@@ -72394,7 +72394,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1468" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1468" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1468" s="19" t="s">
         <v>1464</v>
       </c>
@@ -72498,7 +72498,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1472" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1472" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1472" s="19" t="s">
         <v>421</v>
       </c>
@@ -72576,7 +72576,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1475" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1475" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1475" s="19" t="s">
         <v>2338</v>
       </c>
@@ -72602,7 +72602,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1476" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1476" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1476" s="19" t="s">
         <v>2344</v>
       </c>
@@ -72706,7 +72706,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1480" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1480" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1480" s="19" t="s">
         <v>2383</v>
       </c>
@@ -72732,7 +72732,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1481" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1481" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1481" s="19" t="s">
         <v>209</v>
       </c>
@@ -72758,7 +72758,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1482" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1482" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1482" s="19" t="s">
         <v>208</v>
       </c>
@@ -72836,7 +72836,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1485" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1485" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1485" s="19" t="s">
         <v>412</v>
       </c>
@@ -72862,7 +72862,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1486" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1486" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1486" s="19" t="s">
         <v>2249</v>
       </c>
@@ -72888,7 +72888,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="1487" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1487" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1487" s="19" t="s">
         <v>1561</v>
       </c>
@@ -72914,7 +72914,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1488" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1488" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1488" s="19" t="s">
         <v>1562</v>
       </c>
@@ -72940,7 +72940,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1489" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1489" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1489" s="19" t="s">
         <v>1563</v>
       </c>
@@ -72966,7 +72966,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1490" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1490" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1490" s="19" t="s">
         <v>1564</v>
       </c>
@@ -72992,7 +72992,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1491" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1491" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1491" s="19" t="s">
         <v>1565</v>
       </c>
@@ -73018,7 +73018,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1492" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1492" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1492" s="19" t="s">
         <v>1566</v>
       </c>
@@ -73044,7 +73044,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1493" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1493" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1493" s="19" t="s">
         <v>1567</v>
       </c>
@@ -73070,7 +73070,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1494" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1494" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1494" s="19" t="s">
         <v>1568</v>
       </c>
@@ -73096,7 +73096,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1495" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1495" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1495" s="19" t="s">
         <v>1569</v>
       </c>
@@ -73122,7 +73122,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1496" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1496" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1496" s="19" t="s">
         <v>1570</v>
       </c>
@@ -73148,7 +73148,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1497" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1497" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1497" s="19" t="s">
         <v>1571</v>
       </c>
@@ -73174,7 +73174,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1498" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1498" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1498" s="19" t="s">
         <v>1572</v>
       </c>
@@ -73200,7 +73200,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1499" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1499" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1499" s="19" t="s">
         <v>1586</v>
       </c>
@@ -73226,7 +73226,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1500" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1500" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1500" s="19" t="s">
         <v>1587</v>
       </c>
@@ -73252,7 +73252,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1501" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1501" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1501" s="19" t="s">
         <v>1588</v>
       </c>
@@ -73278,7 +73278,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1502" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1502" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1502" s="19" t="s">
         <v>1589</v>
       </c>
@@ -73304,7 +73304,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1503" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1503" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1503" s="19" t="s">
         <v>1552</v>
       </c>
@@ -73342,7 +73342,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1504" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1504" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1504" s="19" t="s">
         <v>1551</v>
       </c>
@@ -73380,7 +73380,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1505" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1505" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1505" s="19" t="s">
         <v>1531</v>
       </c>
@@ -73415,7 +73415,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1506" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1506" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1506" s="19" t="s">
         <v>1537</v>
       </c>
@@ -73450,7 +73450,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1507" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1507" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1507" s="19" t="s">
         <v>1545</v>
       </c>
@@ -73485,7 +73485,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1508" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1508" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1508" s="19" t="s">
         <v>1541</v>
       </c>
@@ -73520,7 +73520,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1509" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1509" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1509" s="19" t="s">
         <v>1529</v>
       </c>
@@ -73552,7 +73552,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1510" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1510" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1510" s="19" t="s">
         <v>1535</v>
       </c>
@@ -73584,7 +73584,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1511" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1511" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1511" s="19" t="s">
         <v>1111</v>
       </c>
@@ -73613,7 +73613,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1512" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1512" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1512" s="19" t="s">
         <v>900</v>
       </c>
@@ -73642,7 +73642,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1513" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1513" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1513" s="19" t="s">
         <v>1117</v>
       </c>
@@ -73674,7 +73674,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1514" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1514" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1514" s="19" t="s">
         <v>1110</v>
       </c>
@@ -73706,7 +73706,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1515" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1515" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1515" s="19" t="s">
         <v>1113</v>
       </c>
@@ -73738,7 +73738,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1516" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1516" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1516" s="19" t="s">
         <v>1106</v>
       </c>
@@ -73770,7 +73770,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1517" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1517" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1517" s="19" t="s">
         <v>1533</v>
       </c>
@@ -73802,7 +73802,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1518" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1518" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1518" s="19" t="s">
         <v>1116</v>
       </c>
@@ -73834,7 +73834,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1519" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1519" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1519" s="19" t="s">
         <v>1109</v>
       </c>
@@ -73866,7 +73866,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1520" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1520" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1520" s="19" t="s">
         <v>1539</v>
       </c>
@@ -73898,7 +73898,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1521" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1521" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1521" s="19" t="s">
         <v>1547</v>
       </c>
@@ -73930,7 +73930,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1522" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1522" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1522" s="19" t="s">
         <v>1548</v>
       </c>
@@ -73962,7 +73962,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1523" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1523" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1523" s="19" t="s">
         <v>1543</v>
       </c>
@@ -73994,7 +73994,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1524" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1524" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1524" s="19" t="s">
         <v>1549</v>
       </c>
@@ -74026,7 +74026,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1525" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1525" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1525" s="19" t="s">
         <v>1112</v>
       </c>
@@ -74058,7 +74058,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1526" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1526" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1526" s="19" t="s">
         <v>901</v>
       </c>
@@ -74090,7 +74090,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1527" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1527" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1527" s="19" t="s">
         <v>1114</v>
       </c>
@@ -74122,7 +74122,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1528" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1528" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1528" s="19" t="s">
         <v>1107</v>
       </c>
@@ -74154,7 +74154,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1529" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1529" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1529" s="19" t="s">
         <v>1115</v>
       </c>
@@ -74187,7 +74187,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1530" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1530" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1530" s="19" t="s">
         <v>1108</v>
       </c>
@@ -74220,7 +74220,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1531" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1531" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1531" s="19" t="s">
         <v>1573</v>
       </c>
@@ -74246,7 +74246,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1532" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1532" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1532" s="19" t="s">
         <v>1574</v>
       </c>
@@ -74272,7 +74272,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1533" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1533" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1533" s="19" t="s">
         <v>1575</v>
       </c>
@@ -74298,7 +74298,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1534" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1534" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1534" s="19" t="s">
         <v>1576</v>
       </c>
@@ -74324,7 +74324,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1535" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1535" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1535" s="19" t="s">
         <v>1577</v>
       </c>
@@ -74350,7 +74350,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1536" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1536" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1536" s="19" t="s">
         <v>1614</v>
       </c>
@@ -74376,7 +74376,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1537" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1537" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1537" s="19" t="s">
         <v>1606</v>
       </c>
@@ -74405,7 +74405,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1538" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1538" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1538" s="19" t="s">
         <v>1607</v>
       </c>
@@ -74434,7 +74434,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1539" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1539" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1539" s="19" t="s">
         <v>1608</v>
       </c>
@@ -74463,7 +74463,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1540" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1540" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1540" s="19" t="s">
         <v>1609</v>
       </c>
@@ -74492,7 +74492,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1541" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1541" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1541" s="19" t="s">
         <v>1610</v>
       </c>
@@ -74521,7 +74521,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1542" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1542" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1542" s="19" t="s">
         <v>1611</v>
       </c>
@@ -74550,7 +74550,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1543" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1543" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1543" s="19" t="s">
         <v>1612</v>
       </c>
@@ -74579,7 +74579,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1544" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1544" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1544" s="19" t="s">
         <v>1613</v>
       </c>
@@ -74608,7 +74608,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1545" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1545" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1545" s="19" t="s">
         <v>1590</v>
       </c>
@@ -74634,7 +74634,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1546" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1546" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1546" s="19" t="s">
         <v>1591</v>
       </c>
@@ -74660,7 +74660,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1547" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1547" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1547" s="19" t="s">
         <v>1592</v>
       </c>
@@ -74686,7 +74686,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1548" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1548" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1548" s="19" t="s">
         <v>1593</v>
       </c>
@@ -74712,7 +74712,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1549" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1549" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1549" s="19" t="s">
         <v>1594</v>
       </c>
@@ -74738,7 +74738,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1550" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1550" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1550" s="19" t="s">
         <v>1595</v>
       </c>
@@ -74764,7 +74764,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1551" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1551" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1551" s="19" t="s">
         <v>1596</v>
       </c>
@@ -74790,7 +74790,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1552" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1552" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1552" s="19" t="s">
         <v>1597</v>
       </c>
@@ -74816,7 +74816,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1553" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1553" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1553" s="19" t="s">
         <v>1623</v>
       </c>
@@ -74849,7 +74849,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1554" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1554" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1554" s="19" t="s">
         <v>1622</v>
       </c>
@@ -74891,7 +74891,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1555" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1555" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1555" s="19" t="s">
         <v>1598</v>
       </c>
@@ -74920,7 +74920,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1556" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1556" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1556" s="19" t="s">
         <v>1599</v>
       </c>
@@ -74949,7 +74949,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1557" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1557" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1557" s="19" t="s">
         <v>1600</v>
       </c>
@@ -74978,7 +74978,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1558" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1558" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1558" s="19" t="s">
         <v>1601</v>
       </c>
@@ -75007,7 +75007,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1559" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1559" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1559" s="19" t="s">
         <v>1602</v>
       </c>
@@ -75036,7 +75036,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1560" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1560" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1560" s="19" t="s">
         <v>1603</v>
       </c>
@@ -75065,7 +75065,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1561" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1561" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1561" s="19" t="s">
         <v>1604</v>
       </c>
@@ -75094,7 +75094,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1562" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1562" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1562" s="19" t="s">
         <v>1605</v>
       </c>
@@ -75123,7 +75123,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1563" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1563" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1563" s="19" t="s">
         <v>1532</v>
       </c>
@@ -75155,7 +75155,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1564" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1564" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1564" s="19" t="s">
         <v>1538</v>
       </c>
@@ -75187,7 +75187,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1565" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1565" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1565" s="19" t="s">
         <v>1546</v>
       </c>
@@ -75219,7 +75219,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1566" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1566" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1566" s="19" t="s">
         <v>1542</v>
       </c>
@@ -75251,7 +75251,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1567" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1567" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1567" s="19" t="s">
         <v>2308</v>
       </c>
@@ -75283,7 +75283,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1568" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1568" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1568" s="19" t="s">
         <v>1530</v>
       </c>
@@ -75318,7 +75318,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1569" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1569" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1569" s="19" t="s">
         <v>1536</v>
       </c>
@@ -75353,7 +75353,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1570" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1570" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1570" s="19" t="s">
         <v>1544</v>
       </c>
@@ -75388,7 +75388,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1571" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1571" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1571" s="19" t="s">
         <v>1540</v>
       </c>
@@ -75423,7 +75423,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1572" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1572" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1572" s="19" t="s">
         <v>1528</v>
       </c>
@@ -75455,7 +75455,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1573" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1573" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1573" s="19" t="s">
         <v>1534</v>
       </c>
@@ -75487,7 +75487,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1574" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1574" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1574" s="19" t="s">
         <v>1578</v>
       </c>
@@ -75513,7 +75513,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1575" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1575" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1575" s="19" t="s">
         <v>1579</v>
       </c>
@@ -75539,7 +75539,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1576" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1576" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1576" s="19" t="s">
         <v>1580</v>
       </c>
@@ -75565,7 +75565,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1577" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1577" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1577" s="19" t="s">
         <v>1581</v>
       </c>
@@ -75591,7 +75591,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1578" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1578" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1578" s="19" t="s">
         <v>1582</v>
       </c>
@@ -75617,7 +75617,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1579" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1579" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1579" s="19" t="s">
         <v>1583</v>
       </c>
@@ -75643,7 +75643,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1580" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1580" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1580" s="19" t="s">
         <v>1584</v>
       </c>
@@ -75669,7 +75669,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="1581" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1581" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1581" s="19" t="s">
         <v>1585</v>
       </c>
@@ -75699,18 +75699,7 @@
       <c r="A1582"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB1581">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="*"/>
-        <filter val="H"/>
-        <filter val="SH"/>
-        <filter val="SHL"/>
-        <filter val="SHLM"/>
-        <filter val="SHM"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AB1581"/>
   <sortState ref="A2:AB1580">
     <sortCondition ref="AA2:AA1580"/>
     <sortCondition ref="AB2:AB1580"/>
@@ -75718,7 +75707,7 @@
   </sortState>
   <phoneticPr fontId="3"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P859:P869 P1166:P1172 P206 P126:P129 P134:P136 P138:P139 P141:P143 P121:P122 P112:P119 P157:P173 P175:P181 P148:P155 P146 P242:P243 P240 P238 P235 P229:P230 P222:P226 P217 P215 P787:P818 P1466:P1484 P1145:P1159 G1136:G1137 P544:P554 P369:P385 P354:P365 P1199:P1204 G1443:G1484 P1444:P1464 P303:P350 P1089:P1108 P1175:P1189 P289 F1061 P247 P400:P435 P508:P519 P822:P829 P447:P462 F782:F832 P833:P852 H291:H294 P1048:P1083 J295:J386 F291:F293 H387:H398 H1439:I1440 P556:P567 F1118:G1120 P1332:P1359 H4:H5 F2:J3 J6 H7 J1377:J1438 P1377:P1438 F1441:F1486 G1441 F1377:H1438 F6:H6 F1062:H1113 F295:H386 P1003:P1004 P618:P660 F618:G647 G648:G677 F649:F677 P742:P752 P699:P731 P924:P953 P966:P999 F834:F891 P872:P891 P570:P601 H1136:H1138 J399:J567 P468:P475 P480:P503 J570:J903 P664:P696 P523:P539 P762:P780 P782 P1206:P1330 F1132:H1135 P898:P903 P906:P911 H904:H905 J253:J293 H1360:H1376 I253:I1438 F1139:H1359 J1139:J1359 P1195:P1196 P1123:P1137 F1123:G1131 J1118:J1137 H1114:H1131 P1007:P1012 H1441:J1486 F906:H1059 F892:H903 F399:H567 F570:H617 F678:H781 G782:H891 H618:H677 G1060:H1061 H568:H569 J906:J1113 I4:I250 J8:J250 F8:H250 F253:H290 F251:J252 F1487:J1581 P251:P253 P1487:P1575"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P859:P869 P1166:P1172 P206 P126:P129 P134:P136 P138:P139 P141:P143 P121:P122 P112:P119 P157:P173 P175:P181 P148:P155 P146 P242:P243 P240 P238 P235 P229:P230 P222:P226 P217 P215 P787:P818 P1466:P1484 P1145:P1159 G1136:G1137 P544:P554 P369:P385 P354:P365 P1199:P1204 G1443:G1484 P1444:P1464 P303:P350 P1089:P1108 P1175:P1189 P289 F1061 P247 P400:P435 P508:P519 P822:P829 P447:P462 F782:F832 P833:P852 H291:H294 P1048:P1083 J295:J386 F291:F293 H387:H398 H1439:I1440 P556:P567 F1118:G1120 P1332:P1359 H4:H5 F2:J3 J6 H7 J1377:J1438 P1377:P1438 F1441:F1486 G1441 F1377:H1438 F6:H6 F1062:H1113 F295:H386 P1003:P1004 P618:P660 F618:G647 G648:G677 F649:F677 P742:P752 P699:P731 P924:P953 P966:P999 F834:F891 P872:P891 P570:P601 H1136:H1138 J399:J567 P468:P475 P480:P503 J570:J903 P664:P696 P523:P539 P762:P780 P782 P1206:P1330 F1132:H1135 P898:P903 P906:P911 H904:H905 J253:J293 H1360:H1376 I253:I1438 F1139:H1359 P1487:P1575 P1195:P1196 P1123:P1137 F1123:G1131 J1118:J1137 H1114:H1131 P1007:P1012 H1441:J1486 F906:H1059 F892:H903 F399:H567 F570:H617 F678:H781 G782:H891 H618:H677 G1060:H1061 H568:H569 J906:J1113 I4:I250 J8:J250 F8:H250 F253:H290 F251:J252 F1487:J1581 P251:P253 J1139:J1359"/>
   </dataValidations>
   <pageMargins left="0.38" right="0" top="0" bottom="0.2" header="0" footer="0"/>
   <pageSetup scale="60" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Added glyphs needed for Harmattan for cv12 and cv48
</commit_message>
<xml_diff>
--- a/absGlyphList/absGlyphList.xlsx
+++ b/absGlyphList/absGlyphList.xlsx
@@ -16033,10 +16033,10 @@
   <dimension ref="A1:AB1642"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1329" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="A1354" sqref="A1354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -35412,7 +35412,7 @@
         <v>504</v>
       </c>
       <c r="J507" s="11" t="s">
-        <v>2243</v>
+        <v>561</v>
       </c>
       <c r="K507" s="19" t="s">
         <v>4831</v>
@@ -36691,7 +36691,7 @@
         <v>536</v>
       </c>
       <c r="J539" s="11" t="s">
-        <v>2243</v>
+        <v>561</v>
       </c>
       <c r="K539" s="19" t="s">
         <v>4831</v>
@@ -37016,7 +37016,7 @@
         <v>544</v>
       </c>
       <c r="J547" s="11" t="s">
-        <v>2243</v>
+        <v>561</v>
       </c>
       <c r="K547" s="19" t="s">
         <v>4831</v>
@@ -55559,7 +55559,7 @@
         <v>993</v>
       </c>
       <c r="J996" s="11" t="s">
-        <v>2253</v>
+        <v>2252</v>
       </c>
       <c r="K996" t="s">
         <v>1281</v>
@@ -55650,7 +55650,7 @@
         <v>995</v>
       </c>
       <c r="J998" s="11" t="s">
-        <v>2253</v>
+        <v>2252</v>
       </c>
       <c r="U998" t="s">
         <v>1449</v>
@@ -55688,7 +55688,7 @@
         <v>996</v>
       </c>
       <c r="J999" s="11" t="s">
-        <v>2253</v>
+        <v>2252</v>
       </c>
       <c r="U999" t="s">
         <v>1448</v>
@@ -55723,7 +55723,7 @@
         <v>997</v>
       </c>
       <c r="J1000" s="11" t="s">
-        <v>2253</v>
+        <v>2252</v>
       </c>
       <c r="K1000" t="s">
         <v>495</v>
@@ -55767,7 +55767,7 @@
         <v>998</v>
       </c>
       <c r="J1001" s="11" t="s">
-        <v>2253</v>
+        <v>2252</v>
       </c>
       <c r="K1001" t="s">
         <v>1257</v>
@@ -55808,7 +55808,7 @@
         <v>999</v>
       </c>
       <c r="J1002" s="11" t="s">
-        <v>2253</v>
+        <v>2252</v>
       </c>
       <c r="K1002" t="s">
         <v>22</v>
@@ -63244,7 +63244,7 @@
         <v>1181</v>
       </c>
       <c r="J1185" s="13" t="s">
-        <v>2253</v>
+        <v>2252</v>
       </c>
       <c r="X1185" t="s">
         <v>1511</v>
@@ -77641,7 +77641,7 @@
   </sortState>
   <phoneticPr fontId="3"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P881:P891 P1189:P1195 P206 P126:P129 P134:P136 P138:P139 P141:P143 P121:P122 P112:P119 P157:P173 P175:P181 P148:P155 P146 P249:P250 P247 J1479 P240 P222:P226 P217 P215 P809:P840 P1527:P1545 P1168:P1182 P566:P576 P376:P392 P361:P372 P1222:P1227 G1504:G1545 P1505:P1525 P310:P357 P1111:P1130 P1198:P1212 P296 F1083 P254 P407:P442 P521:P536 P844:P851 P454:P469 F804:F854 P855:P874 H298:H301 P1070:P1105 J1502:J1547 F298:F300 H394:H405 P1479 P578:P589 F1140:G1142 P1355:P1382 H4:H5 F2:J3 J6 H7 J1465:J1468 F1502:F1547 G1502 F6:H6 F1084:H1135 F302:H393 P1025:P1026 P640:P682 F640:G669 G670:G699 F671:F699 P764:P774 P721:P753 P946:P975 P988:P1021 F856:F913 P894:P913 P592:P623 J928:J1135 P475:P482 P487:P515 P686:P718 P541:P561 P784:P802 P804 P1229:P1353 F1154:H1157 P920:P925 P928:P933 H926:I927 J1140:J1160 F1162:H1382 P1548:P1636 P1218:P1219 F1145:G1153 H1136:H1153 P1029:P1034 F914:H925 F406:H589 F592:H639 F700:H803 G804:H913 H640:H699 G1082:I1083 H590:I591 J406:J589 F242:H242 F1548:J1642 P258:P260 P237 I4:I589 F8:H228 J8:J228 H1480:H1481 J242 P230 J1400:J1447 J1449:J1457 P1400:P1447 P1449:P1457 J1398 J240 P1465:P1468 J230:J237 P233 F240:H240 F1465:H1468 F1449:H1457 F1400:H1447 F230:H237 H1502:H1547 F1479:H1479 F246:H297 J302:J393 G1158:G1160 F928:I1081 H1383:H1399 I1084:I1547 I592:J925 P1145:P1160 H1158:H1161 J1162:J1382 J1388 J246:J300"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P881:P891 P1189:P1195 P206 P126:P129 P134:P136 P138:P139 P141:P143 P121:P122 P112:P119 P157:P173 P175:P181 P148:P155 P146 P249:P250 P247 J1479 P240 P222:P226 P217 P215 P809:P840 P1527:P1545 P1168:P1182 P566:P576 P376:P392 P361:P372 P1222:P1227 G1504:G1545 P1505:P1525 P310:P357 P1111:P1130 P1198:P1212 P296 F1083 P254 P407:P442 P521:P536 P844:P851 P454:P469 F804:F854 P855:P874 H298:H301 P1070:P1105 J1502:J1547 F298:F300 H394:H405 P1479 P578:P589 F1140:G1142 P1355:P1382 H4:H5 F2:J3 J6 H7 J1465:J1468 F1502:F1547 G1502 F6:H6 F1084:H1135 F302:H393 P1025:P1026 P640:P682 F640:G669 G670:G699 F671:F699 P764:P774 P721:P753 P946:P975 P988:P1021 F856:F913 P894:P913 P592:P623 J246:J300 P475:P482 P487:P515 P686:P718 P541:P561 P784:P802 P804 P1229:P1353 F1154:H1157 P920:P925 P928:P933 H926:I927 J1140:J1160 F1162:H1382 P1548:P1636 P1218:P1219 F1145:G1153 H1136:H1153 P1029:P1034 F914:H925 F406:H589 F592:H639 F700:H803 G804:H913 H640:H699 G1082:I1083 H590:I591 J406:J589 F242:H242 F1548:J1642 P258:P260 P237 I4:I589 F8:H228 J8:J228 H1480:H1481 J242 P230 J1400:J1447 J1449:J1457 P1400:P1447 P1449:P1457 J1398 J240 P1465:P1468 J230:J237 P233 F240:H240 F1465:H1468 F1449:H1457 F1400:H1447 F230:H237 H1502:H1547 F1479:H1479 F246:H297 J302:J393 G1158:G1160 F928:I1081 H1383:H1399 I1084:I1547 I592:J925 P1145:P1160 H1158:H1161 J1162:J1382 J1388 J928:J1135"/>
   </dataValidations>
   <pageMargins left="0.38" right="0" top="0" bottom="0.2" header="0" footer="0"/>
   <pageSetup scale="60" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
I reviewed SenAjami3 and realized Wolof also uses cv74=1 "inverted damma=hollow" so I added the glyph needed for that.
</commit_message>
<xml_diff>
--- a/absGlyphList/absGlyphList.xlsx
+++ b/absGlyphList/absGlyphList.xlsx
@@ -16033,10 +16033,10 @@
   <dimension ref="A1:AB1642"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1329" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B1171" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1354" sqref="A1354"/>
+      <selection pane="bottomRight" activeCell="J1197" sqref="J1197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -63660,7 +63660,7 @@
         <v>1193</v>
       </c>
       <c r="J1197" s="11" t="s">
-        <v>572</v>
+        <v>2244</v>
       </c>
       <c r="X1197" t="s">
         <v>1520</v>

</xml_diff>